<commit_message>
modified my_vids.txt products.py nfreqs.xlsx MinorScales.xlsx
</commit_message>
<xml_diff>
--- a/MinorScales.xlsx
+++ b/MinorScales.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="300" windowWidth="18816" windowHeight="9432"/>
@@ -192,8 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +253,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -331,6 +336,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -365,6 +371,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,20 +547,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="26" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>50</v>
       </c>
@@ -606,7 +613,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <v>0</v>
       </c>
@@ -647,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -691,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -735,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -779,7 +786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -823,7 +830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -867,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -896,7 +903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -940,7 +947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -969,7 +976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1099,12 +1106,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1151,7 +1158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1245,7 +1252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1386,7 +1393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1433,12 +1440,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1532,7 +1539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1626,7 +1633,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1673,7 +1680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -1767,12 +1774,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -1819,7 +1826,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -1866,7 +1873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
@@ -1913,7 +1920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -2054,7 +2061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -2101,12 +2108,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -2153,7 +2160,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -2247,7 +2254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -2294,7 +2301,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -2341,7 +2348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -2435,12 +2442,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>20</v>
       </c>
@@ -2534,7 +2541,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
@@ -2581,7 +2588,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -2628,7 +2635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -2675,7 +2682,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
@@ -2722,7 +2729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>18</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>47</v>
       </c>
@@ -2816,7 +2823,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>26</v>
       </c>
@@ -2863,7 +2870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>30</v>
       </c>
@@ -2910,7 +2917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>29</v>
       </c>
@@ -2957,7 +2964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>27</v>
       </c>
@@ -3051,7 +3058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>15</v>
       </c>
@@ -3098,7 +3105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
@@ -3145,7 +3152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -3193,24 +3200,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>